<commit_message>
Add rules for 78
</commit_message>
<xml_diff>
--- a/runtime_dev/apps/delphes/delphes.xlsx
+++ b/runtime_dev/apps/delphes/delphes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joel/Documents/Dev/Athena/trusted-service/runtime_dev/apps/delphes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{783734B1-3E6A-8841-926A-EE04FA830198}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74382A74-88B3-994E-8740-881D8FE2D379}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18860" tabRatio="973" firstSheet="3" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18860" tabRatio="973" firstSheet="4" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="APP &amp; MODEL" sheetId="25" r:id="rId1"/>
@@ -18,20 +18,19 @@
     <sheet name="localized_app" sheetId="14" r:id="rId3"/>
     <sheet name="messages_to_agent" sheetId="21" r:id="rId4"/>
     <sheet name="messages_to_requester" sheetId="20" r:id="rId5"/>
-    <sheet name="Feuil1" sheetId="31" r:id="rId6"/>
-    <sheet name="case_fields" sheetId="10" r:id="rId7"/>
-    <sheet name="TEXT ANALYSIS" sheetId="26" r:id="rId8"/>
-    <sheet name="text_analysis" sheetId="1" r:id="rId9"/>
-    <sheet name="definitions" sheetId="7" r:id="rId10"/>
-    <sheet name="intentions" sheetId="2" r:id="rId11"/>
-    <sheet name="DECISION" sheetId="27" r:id="rId12"/>
-    <sheet name="decision_engine_configs" sheetId="29" r:id="rId13"/>
-    <sheet name="DISTRIBUTION" sheetId="28" r:id="rId14"/>
-    <sheet name="email_config" sheetId="13" r:id="rId15"/>
-    <sheet name="email_templates" sheetId="11" r:id="rId16"/>
-    <sheet name="APP-SPECIFIC" sheetId="22" r:id="rId17"/>
-    <sheet name="statuts" sheetId="30" r:id="rId18"/>
-    <sheet name="arrondissements" sheetId="23" r:id="rId19"/>
+    <sheet name="case_fields" sheetId="10" r:id="rId6"/>
+    <sheet name="TEXT ANALYSIS" sheetId="26" r:id="rId7"/>
+    <sheet name="text_analysis" sheetId="1" r:id="rId8"/>
+    <sheet name="definitions" sheetId="7" r:id="rId9"/>
+    <sheet name="intentions" sheetId="2" r:id="rId10"/>
+    <sheet name="DECISION" sheetId="27" r:id="rId11"/>
+    <sheet name="decision_engine_configs" sheetId="29" r:id="rId12"/>
+    <sheet name="DISTRIBUTION" sheetId="28" r:id="rId13"/>
+    <sheet name="email_config" sheetId="13" r:id="rId14"/>
+    <sheet name="email_templates" sheetId="11" r:id="rId15"/>
+    <sheet name="APP-SPECIFIC" sheetId="22" r:id="rId16"/>
+    <sheet name="statuts" sheetId="30" r:id="rId17"/>
+    <sheet name="arrondissements" sheetId="23" r:id="rId18"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -54,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="659" uniqueCount="397">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="693" uniqueCount="407">
   <si>
     <t>Parameter</t>
   </si>
@@ -1175,45 +1174,30 @@
     <t>rdv_remise_de_titre</t>
   </si>
   <si>
-    <t>PRISE DE RENDEZ_VOUS REMISE DE TITRES</t>
-  </si>
-  <si>
     <t>Le demandeur demande un rendez-vous pour une remise de titre</t>
   </si>
   <si>
     <t>rdv_renouvellement_recepisse</t>
   </si>
   <si>
-    <t>PRISE DE RENDEZ_VOUS RENOUVELLEMENT RECEPISSE</t>
-  </si>
-  <si>
     <t>Le demandeur demande un rendez-vous pour le renouvellement de son récépissé</t>
   </si>
   <si>
     <t>rdv_renouvellement_titre_sejour_hors_anef</t>
   </si>
   <si>
-    <t>PRISE DE RENDEZ_VOUS RENOUVELLEMENT DE TITRE DE SEJOUR HORS ANEF</t>
-  </si>
-  <si>
     <t>Le demandeur demande un rendez-vous pour le renouvellement d'un titre de séjour. Sa demande s'inscrit dans un processus géré en dehors du site de l'anef</t>
   </si>
   <si>
     <t>rdv_sauf_conduit</t>
   </si>
   <si>
-    <t>PRISE DE RENDEZ_VOUS SAUF-CONDUITS</t>
-  </si>
-  <si>
     <t>Le demandeur demande un rendez-vous pour un sauf-conduit</t>
   </si>
   <si>
     <t>rdv_premiere_demande_titre_sejour</t>
   </si>
   <si>
-    <t>PRISE DE RENDEZ_VOUS PREMIERE DEMANDE DE TITRE DE SEJOUR</t>
-  </si>
-  <si>
     <t>Le demandeur demande un rendez-vous pour une première demande de titre de séjour</t>
   </si>
   <si>
@@ -1293,15 +1277,67 @@
   </si>
   <si>
     <t>Please go to the reception desk at the prefecture to make this request in person.</t>
+  </si>
+  <si>
+    <t>date_expiration_recepisse</t>
+  </si>
+  <si>
+    <t>Acknowledgement document expiry date (DD/MM/YYYY)</t>
+  </si>
+  <si>
+    <t>Date d'expiration du récépissé au format JJ/MM/AAAA</t>
+  </si>
+  <si>
+    <t>Acknowledgement document expiration date formatted as DD/MM/YYYY</t>
+  </si>
+  <si>
+    <t>date d'expiration du récépissé au format JJ/MM/AAAA</t>
+  </si>
+  <si>
+    <t>date_expiration_titre_sejour</t>
+  </si>
+  <si>
+    <t>Resident permit expiry date (DD/MM/YYYY)</t>
+  </si>
+  <si>
+    <t>Date d'expiration du titre de séjour au format JJ/MM/AAAA</t>
+  </si>
+  <si>
+    <t>Resident permit expiration date formatted as DD/MM/YYYY</t>
+  </si>
+  <si>
+    <t>date d'expiration du titre de séjour au format JJ/MM/AAAA</t>
+  </si>
+  <si>
+    <t>PRISE DE RENDEZ-VOUS PREMIERE DEMANDE DE TITRE DE SEJOUR</t>
+  </si>
+  <si>
+    <t>PRISE DE RENDEZ-VOUS SAUF-CONDUITS</t>
+  </si>
+  <si>
+    <t>PRISE DE RENDEZ-VOUS RENOUVELLEMENT DE TITRE DE SEJOUR HORS ANEF</t>
+  </si>
+  <si>
+    <t>PRISE DE RENDEZ-VOUS RENOUVELLEMENT RECEPISSE</t>
+  </si>
+  <si>
+    <t>PRISE DE RENDEZ-VOUS REMISE DE TITRES</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1416,10 +1452,10 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1427,24 +1463,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="2" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="2" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="2" quotePrefix="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
@@ -1452,21 +1488,21 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1475,8 +1511,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1776,98 +1818,11 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F212B83-BB31-486E-8D1E-C153171C389E}">
-  <dimension ref="A1:C6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="45.6640625" customWidth="1"/>
-    <col min="2" max="2" width="90.1640625" customWidth="1"/>
-    <col min="3" max="3" width="108.33203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="48" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="28" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>221</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>150</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40884519-E9E2-4702-AA20-B46B229B9942}">
   <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25:A30"/>
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2240,10 +2195,10 @@
         <v>353</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>371</v>
+        <v>366</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>372</v>
+        <v>367</v>
       </c>
       <c r="D25" s="24" t="s">
         <v>354</v>
@@ -2257,84 +2212,84 @@
         <v>356</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>373</v>
+        <v>368</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>374</v>
-      </c>
-      <c r="D26" s="24" t="s">
+        <v>369</v>
+      </c>
+      <c r="D26" s="31" t="s">
+        <v>406</v>
+      </c>
+      <c r="E26" s="24" t="s">
         <v>357</v>
-      </c>
-      <c r="E26" s="24" t="s">
-        <v>358</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A27" s="29" t="s">
+        <v>358</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>370</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>371</v>
+      </c>
+      <c r="D27" s="31" t="s">
+        <v>405</v>
+      </c>
+      <c r="E27" s="24" t="s">
         <v>359</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>375</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>376</v>
-      </c>
-      <c r="D27" s="24" t="s">
-        <v>360</v>
-      </c>
-      <c r="E27" s="24" t="s">
-        <v>361</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A28" s="29" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>377</v>
+        <v>372</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>378</v>
-      </c>
-      <c r="D28" s="24" t="s">
-        <v>363</v>
+        <v>373</v>
+      </c>
+      <c r="D28" s="31" t="s">
+        <v>404</v>
       </c>
       <c r="E28" s="24" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A29" s="29" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>379</v>
+        <v>374</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>380</v>
-      </c>
-      <c r="D29" s="24" t="s">
-        <v>366</v>
+        <v>375</v>
+      </c>
+      <c r="D29" s="31" t="s">
+        <v>403</v>
       </c>
       <c r="E29" s="24" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A30" s="29" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>381</v>
+        <v>376</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>381</v>
-      </c>
-      <c r="D30" s="24" t="s">
-        <v>369</v>
+        <v>376</v>
+      </c>
+      <c r="D30" s="31" t="s">
+        <v>402</v>
       </c>
       <c r="E30" s="24" t="s">
-        <v>370</v>
+        <v>365</v>
       </c>
     </row>
   </sheetData>
@@ -2343,7 +2298,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A5987CB-B31E-4266-A5A3-C356313D0A31}">
   <sheetPr>
     <tabColor theme="4"/>
@@ -2360,7 +2315,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B94FBD62-D62F-48D9-8AC0-E46102572B8C}">
   <dimension ref="A1:F4"/>
   <sheetViews>
@@ -2468,7 +2423,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C421946-477F-451E-AF1F-9EE7DF5B81A2}">
   <sheetPr>
     <tabColor theme="4"/>
@@ -2485,7 +2440,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AD020DE-44B7-44EF-BEA3-8491F2595E0A}">
   <dimension ref="A1:C8"/>
   <sheetViews>
@@ -2525,7 +2480,7 @@
         <v>93</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>387</v>
+        <v>382</v>
       </c>
       <c r="C3" s="2"/>
     </row>
@@ -2585,7 +2540,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAADDD23-DB13-4EC8-8D22-BE27FCA5478C}">
   <dimension ref="A1:E4"/>
   <sheetViews>
@@ -2675,7 +2630,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F8AFBFA-5790-4484-BB1A-96526826C9C1}">
   <sheetPr>
     <tabColor theme="4"/>
@@ -2692,12 +2647,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3196DC8C-1CF2-1843-8E1D-27C89DB08A56}">
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView zoomScale="184" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:XFD16"/>
+      <selection activeCell="A2" sqref="A2:A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3004,7 +2959,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{316FA168-2252-420B-B68F-E9525D61AA2D}">
   <dimension ref="A1:H31"/>
   <sheetViews>
@@ -3536,7 +3491,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3566,10 +3521,10 @@
         <v>189</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>391</v>
+        <v>386</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>390</v>
+        <v>385</v>
       </c>
       <c r="D2" s="2"/>
     </row>
@@ -3578,10 +3533,10 @@
         <v>194</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>392</v>
+        <v>387</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>393</v>
+        <v>388</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>196</v>
@@ -3592,22 +3547,22 @@
         <v>193</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
       <c r="D4" s="2"/>
     </row>
     <row r="5" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="28" t="s">
-        <v>388</v>
+        <v>383</v>
       </c>
       <c r="B5" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
       <c r="C5" s="28" t="s">
-        <v>389</v>
+        <v>384</v>
       </c>
     </row>
   </sheetData>
@@ -3617,23 +3572,11 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9F74B94-09A3-594C-94DF-4EC15E7E134C}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF16B1B1-A6B4-4B56-9813-CCF1B731EDAC}">
+  <dimension ref="A1:Q15"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF16B1B1-A6B4-4B56-9813-CCF1B731EDAC}">
-  <dimension ref="A1:Q13"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView topLeftCell="N1" zoomScale="137" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="R15" sqref="R15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4275,8 +4218,8 @@
       <c r="L12" s="8" t="s">
         <v>233</v>
       </c>
-      <c r="M12" s="13" t="s">
-        <v>241</v>
+      <c r="M12" t="s">
+        <v>360</v>
       </c>
       <c r="N12" s="8" t="s">
         <v>241</v>
@@ -4293,16 +4236,16 @@
     </row>
     <row r="13" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="25" t="s">
-        <v>382</v>
+        <v>377</v>
       </c>
       <c r="B13" s="25" t="s">
         <v>5</v>
       </c>
       <c r="C13" s="26" t="s">
-        <v>384</v>
+        <v>379</v>
       </c>
       <c r="D13" s="26" t="s">
-        <v>383</v>
+        <v>378</v>
       </c>
       <c r="E13" s="27" t="s">
         <v>234</v>
@@ -4311,21 +4254,127 @@
         <v>289</v>
       </c>
       <c r="L13" s="27" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="M13" s="23" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="N13" t="s">
-        <v>386</v>
+        <v>381</v>
       </c>
       <c r="O13" s="26" t="s">
-        <v>385</v>
+        <v>380</v>
       </c>
       <c r="P13" s="7" t="s">
         <v>76</v>
       </c>
       <c r="Q13" s="8" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+      <c r="A14" s="17" t="s">
+        <v>392</v>
+      </c>
+      <c r="B14" s="17" t="s">
+        <v>106</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>393</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>394</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>234</v>
+      </c>
+      <c r="F14" s="14" t="s">
+        <v>241</v>
+      </c>
+      <c r="G14" s="14" t="s">
+        <v>241</v>
+      </c>
+      <c r="H14" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="I14" s="14" t="s">
+        <v>241</v>
+      </c>
+      <c r="J14" s="14" t="s">
+        <v>241</v>
+      </c>
+      <c r="K14" s="8" t="s">
+        <v>289</v>
+      </c>
+      <c r="L14" s="8" t="s">
+        <v>233</v>
+      </c>
+      <c r="M14" s="30" t="s">
+        <v>358</v>
+      </c>
+      <c r="N14" s="7" t="s">
+        <v>395</v>
+      </c>
+      <c r="O14" s="7" t="s">
+        <v>396</v>
+      </c>
+      <c r="P14" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="Q14" s="8" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A15" s="17" t="s">
+        <v>397</v>
+      </c>
+      <c r="B15" s="17" t="s">
+        <v>106</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>398</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>399</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>234</v>
+      </c>
+      <c r="F15" s="14" t="s">
+        <v>241</v>
+      </c>
+      <c r="G15" s="14" t="s">
+        <v>241</v>
+      </c>
+      <c r="H15" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="I15" s="14" t="s">
+        <v>241</v>
+      </c>
+      <c r="J15" s="14" t="s">
+        <v>241</v>
+      </c>
+      <c r="K15" s="8" t="s">
+        <v>289</v>
+      </c>
+      <c r="L15" s="8" t="s">
+        <v>233</v>
+      </c>
+      <c r="M15" t="s">
+        <v>360</v>
+      </c>
+      <c r="N15" s="7" t="s">
+        <v>400</v>
+      </c>
+      <c r="O15" s="7" t="s">
+        <v>401</v>
+      </c>
+      <c r="P15" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="Q15" s="8" t="s">
         <v>233</v>
       </c>
     </row>
@@ -4340,7 +4389,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{812DA96A-08DE-4357-A9EB-94B5058F1275}">
   <sheetPr>
     <tabColor theme="4"/>
@@ -4357,7 +4406,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C3"/>
   <sheetViews>
@@ -4406,4 +4455,91 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F212B83-BB31-486E-8D1E-C153171C389E}">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="45.6640625" customWidth="1"/>
+    <col min="2" max="2" width="90.1640625" customWidth="1"/>
+    <col min="3" max="3" width="108.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="48" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="28" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>150</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Frontend: remember form content
</commit_message>
<xml_diff>
--- a/runtime_dev/apps/delphes/delphes.xlsx
+++ b/runtime_dev/apps/delphes/delphes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joel/Documents/Dev/Athena/trusted-service/runtime_dev/apps/delphes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74382A74-88B3-994E-8740-881D8FE2D379}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{743FE121-BEFA-3E45-B0E8-B594C0B7E12A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18860" tabRatio="973" firstSheet="4" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1174,33 +1174,18 @@
     <t>rdv_remise_de_titre</t>
   </si>
   <si>
-    <t>Le demandeur demande un rendez-vous pour une remise de titre</t>
-  </si>
-  <si>
     <t>rdv_renouvellement_recepisse</t>
   </si>
   <si>
-    <t>Le demandeur demande un rendez-vous pour le renouvellement de son récépissé</t>
-  </si>
-  <si>
     <t>rdv_renouvellement_titre_sejour_hors_anef</t>
   </si>
   <si>
-    <t>Le demandeur demande un rendez-vous pour le renouvellement d'un titre de séjour. Sa demande s'inscrit dans un processus géré en dehors du site de l'anef</t>
-  </si>
-  <si>
     <t>rdv_sauf_conduit</t>
   </si>
   <si>
-    <t>Le demandeur demande un rendez-vous pour un sauf-conduit</t>
-  </si>
-  <si>
     <t>rdv_premiere_demande_titre_sejour</t>
   </si>
   <si>
-    <t>Le demandeur demande un rendez-vous pour une première demande de titre de séjour</t>
-  </si>
-  <si>
     <t>DIFFICULTY IN MAKING APPOINTMENTS</t>
   </si>
   <si>
@@ -1249,9 +1234,6 @@
     <t>Safe conduct is requested on grounds of death.</t>
   </si>
   <si>
-    <t>envoishibou78@gmail.com</t>
-  </si>
-  <si>
     <t>ACCUEIL</t>
   </si>
   <si>
@@ -1322,6 +1304,24 @@
   </si>
   <si>
     <t>PRISE DE RENDEZ-VOUS REMISE DE TITRES</t>
+  </si>
+  <si>
+    <t>pocagent78@gmail.com</t>
+  </si>
+  <si>
+    <t>Le demandeur désire prendre un rendez-vous. La raison du rendez-vous est : remise de titre</t>
+  </si>
+  <si>
+    <t>Le demandeur sollicite la prise d'un rendez-vous pour le renouvellement de son récépissé</t>
+  </si>
+  <si>
+    <t>Le demandeur demande à prendre un rendez-vous pour le renouvellement d'un titre de séjour. Sa demande s'inscrit dans un processus géré en dehors du site de l'anef</t>
+  </si>
+  <si>
+    <t>Le demandeur demande à prendre un rendez-vous pour un sauf-conduit</t>
+  </si>
+  <si>
+    <t>Le demandeur demande à prendre un rendez-vous pour une première demande de titre de séjour</t>
   </si>
 </sst>
 </file>
@@ -1822,7 +1822,7 @@
   <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2195,15 +2195,15 @@
         <v>353</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>367</v>
+        <v>362</v>
       </c>
       <c r="D25" s="24" t="s">
         <v>354</v>
       </c>
-      <c r="E25" s="24" t="s">
+      <c r="E25" s="31" t="s">
         <v>355</v>
       </c>
     </row>
@@ -2212,84 +2212,84 @@
         <v>356</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>368</v>
+        <v>363</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>369</v>
+        <v>364</v>
       </c>
       <c r="D26" s="31" t="s">
-        <v>406</v>
-      </c>
-      <c r="E26" s="24" t="s">
-        <v>357</v>
+        <v>400</v>
+      </c>
+      <c r="E26" s="31" t="s">
+        <v>402</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A27" s="29" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>370</v>
+        <v>365</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>371</v>
+        <v>366</v>
       </c>
       <c r="D27" s="31" t="s">
-        <v>405</v>
-      </c>
-      <c r="E27" s="24" t="s">
-        <v>359</v>
+        <v>399</v>
+      </c>
+      <c r="E27" s="31" t="s">
+        <v>403</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A28" s="29" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>372</v>
+        <v>367</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>373</v>
+        <v>368</v>
       </c>
       <c r="D28" s="31" t="s">
+        <v>398</v>
+      </c>
+      <c r="E28" s="31" t="s">
         <v>404</v>
-      </c>
-      <c r="E28" s="24" t="s">
-        <v>361</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A29" s="29" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
       <c r="D29" s="31" t="s">
-        <v>403</v>
-      </c>
-      <c r="E29" s="24" t="s">
-        <v>363</v>
+        <v>397</v>
+      </c>
+      <c r="E29" s="31" t="s">
+        <v>405</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A30" s="29" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>376</v>
+        <v>371</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>376</v>
+        <v>371</v>
       </c>
       <c r="D30" s="31" t="s">
-        <v>402</v>
-      </c>
-      <c r="E30" s="24" t="s">
-        <v>365</v>
+        <v>396</v>
+      </c>
+      <c r="E30" s="31" t="s">
+        <v>406</v>
       </c>
     </row>
   </sheetData>
@@ -2445,7 +2445,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2480,7 +2480,7 @@
         <v>93</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>382</v>
+        <v>401</v>
       </c>
       <c r="C3" s="2"/>
     </row>
@@ -3521,10 +3521,10 @@
         <v>189</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>386</v>
+        <v>380</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>385</v>
+        <v>379</v>
       </c>
       <c r="D2" s="2"/>
     </row>
@@ -3533,10 +3533,10 @@
         <v>194</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>388</v>
+        <v>382</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>196</v>
@@ -3547,22 +3547,22 @@
         <v>193</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>390</v>
+        <v>384</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>389</v>
+        <v>383</v>
       </c>
       <c r="D4" s="2"/>
     </row>
     <row r="5" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="28" t="s">
-        <v>383</v>
+        <v>377</v>
       </c>
       <c r="B5" t="s">
-        <v>391</v>
+        <v>385</v>
       </c>
       <c r="C5" s="28" t="s">
-        <v>384</v>
+        <v>378</v>
       </c>
     </row>
   </sheetData>
@@ -4219,7 +4219,7 @@
         <v>233</v>
       </c>
       <c r="M12" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="N12" s="8" t="s">
         <v>241</v>
@@ -4236,16 +4236,16 @@
     </row>
     <row r="13" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="25" t="s">
-        <v>377</v>
+        <v>372</v>
       </c>
       <c r="B13" s="25" t="s">
         <v>5</v>
       </c>
       <c r="C13" s="26" t="s">
-        <v>379</v>
+        <v>374</v>
       </c>
       <c r="D13" s="26" t="s">
-        <v>378</v>
+        <v>373</v>
       </c>
       <c r="E13" s="27" t="s">
         <v>234</v>
@@ -4257,13 +4257,13 @@
         <v>233</v>
       </c>
       <c r="M13" s="23" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="N13" t="s">
-        <v>381</v>
+        <v>376</v>
       </c>
       <c r="O13" s="26" t="s">
-        <v>380</v>
+        <v>375</v>
       </c>
       <c r="P13" s="7" t="s">
         <v>76</v>
@@ -4274,16 +4274,16 @@
     </row>
     <row r="14" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="17" t="s">
-        <v>392</v>
+        <v>386</v>
       </c>
       <c r="B14" s="17" t="s">
         <v>106</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>393</v>
+        <v>387</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>394</v>
+        <v>388</v>
       </c>
       <c r="E14" s="8" t="s">
         <v>234</v>
@@ -4310,13 +4310,13 @@
         <v>233</v>
       </c>
       <c r="M14" s="30" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="N14" s="7" t="s">
-        <v>395</v>
+        <v>389</v>
       </c>
       <c r="O14" s="7" t="s">
-        <v>396</v>
+        <v>390</v>
       </c>
       <c r="P14" s="7" t="s">
         <v>76</v>
@@ -4327,16 +4327,16 @@
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15" s="17" t="s">
-        <v>397</v>
+        <v>391</v>
       </c>
       <c r="B15" s="17" t="s">
         <v>106</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>398</v>
+        <v>392</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>399</v>
+        <v>393</v>
       </c>
       <c r="E15" s="8" t="s">
         <v>234</v>
@@ -4363,13 +4363,13 @@
         <v>233</v>
       </c>
       <c r="M15" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="N15" s="7" t="s">
-        <v>400</v>
+        <v>394</v>
       </c>
       <c r="O15" s="7" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="P15" s="7" t="s">
         <v>76</v>

</xml_diff>

<commit_message>
fix typo in delphes.xlsx on runtime_dev
</commit_message>
<xml_diff>
--- a/runtime_dev/apps/delphes/delphes.xlsx
+++ b/runtime_dev/apps/delphes/delphes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11018"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11109"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joel/Documents/Dev/Athena/trusted-service/runtime_dev/apps/delphes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4C84CBA-62B5-E34D-B574-C03E9F8E1E19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11E509CE-2EEA-4741-BE64-F21549FC8658}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18860" tabRatio="973" firstSheet="4" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="680" windowWidth="33600" windowHeight="18860" tabRatio="973" firstSheet="3" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="APP &amp; MODEL" sheetId="25" r:id="rId1"/>
@@ -1458,16 +1458,6 @@
   </si>
   <si>
     <t>{prenom} {nom},
-Nous accusons réception de votre demande du {date_demande} concernant l’expiration de votre Autorisation Provisoire de Séjour (API).
-Après examen de votre dossier, nous vous informons que votre demande a été enregistrée et traitée par nos services. Votre situation a bien été prise en compte et les éléments transmis seront intégrés à votre dossier en cours.
-Conformément à la réglementation, vous serez prochainement contacté afin de finaliser la procédure (convocation en préfecture ou communication de la décision administrative). Dans l’attente, il est important de conserver les justificatifs de dépôt ou de renouvellement qui vous ont été remis. Ceux-ci tiennent lieu de preuve de la régularité de votre séjour jusqu’à la notification d’une décision officielle.
-Nous vous invitons à rester attentif aux communications de la préfecture et à consulter régulièrement vos courriels. Pour toute question complémentaire ou en cas de modification de votre situation personnelle, vous pouvez contacter le service des étrangers par courrier électronique à l’adresse suivante : [adresse générique du service] ou par téléphone aux horaires d’accueil indiqués sur notre site.
-Nous vous prions d’agréer, {prenom} {nom}, l’expression de notre considération distinguée.
-Préfecture des Yvelines
-Direction des migrations et de l'intégration</t>
-  </si>
-  <si>
-    <t>{prenom} {nom},
 En réponse à votre demande, je vous invite à nous adresser une copie des éléments suivants :
 - l’acte de décès traduit
 - votre acte de naissance
@@ -1479,34 +1469,113 @@
 Direction des migrations et de l'intégration</t>
   </si>
   <si>
-    <t>{prenom} {nom},
-Nous accusons réception de votre demande du {date_demande} concernant l'expiration de votre Attestation de Demande d’Asile (ATDA).
+    <t>numero_dossier_ANEF</t>
+  </si>
+  <si>
+    <t>Numéro de dossier ANEF</t>
+  </si>
+  <si>
+    <t>ANEF file number</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">{prenom} {nom},
+Nous accusons réception de votre demande du {date_demande} concernant l’expiration de votre </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Autorisation Provisoire d'Instruction</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (API).
+Après examen de votre dossier, nous vous informons que votre demande a été enregistrée et traitée par nos services. Votre situation a bien été prise en compte et les éléments transmis seront intégrés à votre dossier en cours.
+Conformément à la réglementation, vous serez prochainement contacté afin de finaliser la procédure (convocation en préfecture ou communication de la décision administrative). Dans l’attente, il est important de conserver les justificatifs de dépôt ou de renouvellement qui vous ont été remis. Ceux-ci tiennent lieu de preuve de la régularité de votre séjour jusqu’à la notification d’une décision officielle.
+Nous vous invitons à rester attentif aux communications de la préfecture et à consulter régulièrement vos courriels. Pour toute question complémentaire ou en cas de modification de votre situation personnelle, vous pouvez contacter le service des étrangers par courrier électronique à l’adresse suivante : [adresse générique du service] ou par téléphone aux horaires d’accueil indiqués sur notre site.
 Nous vous prions d’agréer, {prenom} {nom}, l’expression de notre considération distinguée.
 Préfecture des Yvelines
 Direction des migrations et de l'intégration</t>
-  </si>
-  <si>
-    <t>{prenom} {nom},
-Nous accusons réception de votre demande du {date_demande} à propos de votre procédure Dublin en cours.
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">{prenom} {nom},
+Nous accusons réception de votre demande du {date_demande} concernant </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>l'expiration de votre Attestation de Demande d’Asile</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (ATDA).
 Nous vous prions d’agréer, {prenom} {nom}, l’expression de notre considération distinguée.
 Préfecture des Yvelines
 Direction des migrations et de l'intégration</t>
-  </si>
-  <si>
-    <t>numero_dossier_ANEF</t>
-  </si>
-  <si>
-    <t>Numéro de dossier ANEF</t>
-  </si>
-  <si>
-    <t>ANEF file number</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">{prenom} {nom},
+Nous accusons réception de votre demande du {date_demande} à propos de votre </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>procédure Dublin</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> en cours.
+Nous vous prions d’agréer, {prenom} {nom}, l’expression de notre considération distinguée.
+Préfecture des Yvelines
+Direction des migrations et de l'intégration</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1566,6 +1635,14 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="7">
@@ -2453,7 +2530,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="68" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A28" s="32" t="s">
         <v>353</v>
       </c>
@@ -2807,8 +2884,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAADDD23-DB13-4EC8-8D22-BE27FCA5478C}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView topLeftCell="B3" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" topLeftCell="C2" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2851,7 +2928,7 @@
         <v>82</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>456</v>
+        <v>460</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="208" x14ac:dyDescent="0.2">
@@ -2868,7 +2945,7 @@
         <v>101</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="160" x14ac:dyDescent="0.2">
@@ -2885,7 +2962,7 @@
         <v>344</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>458</v>
+        <v>461</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="144" x14ac:dyDescent="0.2">
@@ -2902,7 +2979,7 @@
         <v>402</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>459</v>
+        <v>462</v>
       </c>
     </row>
   </sheetData>
@@ -3948,7 +4025,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF16B1B1-A6B4-4B56-9813-CCF1B731EDAC}">
   <dimension ref="A1:Q17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="137" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="C1" zoomScale="137" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="O19" sqref="O19"/>
     </sheetView>
   </sheetViews>
@@ -4796,16 +4873,16 @@
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A17" s="16" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="B17" s="16" t="s">
         <v>4</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
       <c r="E17" s="8" t="s">
         <v>233</v>
@@ -4829,10 +4906,10 @@
         <v>43</v>
       </c>
       <c r="N17" s="7" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="O17" s="7" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
       <c r="P17" s="7" t="s">
         <v>76</v>

</xml_diff>

<commit_message>
Manage intention "autre" (new bannette, new rule)
</commit_message>
<xml_diff>
--- a/runtime_dev/apps/delphes/delphes.xlsx
+++ b/runtime_dev/apps/delphes/delphes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joel/Documents/Dev/Athena/trusted-service/runtime_dev/apps/delphes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11E509CE-2EEA-4741-BE64-F21549FC8658}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{339C7AC1-23D2-BF4C-81ED-12C63B047F98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="680" windowWidth="33600" windowHeight="18860" tabRatio="973" firstSheet="3" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="680" windowWidth="33600" windowHeight="18860" tabRatio="973" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="APP &amp; MODEL" sheetId="25" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="763" uniqueCount="463">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="766" uniqueCount="466">
   <si>
     <t>Parameter</t>
   </si>
@@ -1569,6 +1569,15 @@
 Préfecture des Yvelines
 Direction des migrations et de l'intégration</t>
     </r>
+  </si>
+  <si>
+    <t>INTENTION_AUTRE</t>
+  </si>
+  <si>
+    <t>Le demandeur a sélectionné l'intention "Autre"</t>
+  </si>
+  <si>
+    <t>The applicant has selected the intention "Other"</t>
   </si>
 </sst>
 </file>
@@ -1736,7 +1745,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1803,11 +1812,12 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="2" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="2" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Lien hypertexte" xfId="2" builtinId="8"/>
@@ -2110,7 +2120,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40884519-E9E2-4702-AA20-B46B229B9942}">
   <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
@@ -2625,10 +2635,10 @@
       <c r="C33" s="5" t="s">
         <v>453</v>
       </c>
-      <c r="D33" s="35" t="s">
+      <c r="D33" s="34" t="s">
         <v>450</v>
       </c>
-      <c r="E33" s="35" t="s">
+      <c r="E33" s="34" t="s">
         <v>451</v>
       </c>
     </row>
@@ -2884,7 +2894,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAADDD23-DB13-4EC8-8D22-BE27FCA5478C}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C2" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
@@ -3782,16 +3792,16 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2ED06FD-CD59-4243-896C-6A0821CD9182}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="38.33203125" customWidth="1"/>
-    <col min="2" max="2" width="36" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="46" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3895,14 +3905,25 @@
       </c>
     </row>
     <row r="10" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A10" s="34" t="s">
+      <c r="A10" s="2" t="s">
         <v>441</v>
       </c>
-      <c r="B10" s="25" t="s">
+      <c r="B10" s="7" t="s">
         <v>443</v>
       </c>
-      <c r="C10" s="25" t="s">
+      <c r="C10" s="7" t="s">
         <v>442</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A11" s="36" t="s">
+        <v>463</v>
+      </c>
+      <c r="B11" s="37" t="s">
+        <v>465</v>
+      </c>
+      <c r="C11" s="37" t="s">
+        <v>464</v>
       </c>
     </row>
   </sheetData>
@@ -4382,10 +4403,10 @@
       <c r="E7" s="8" t="s">
         <v>232</v>
       </c>
-      <c r="F7" s="36" t="s">
+      <c r="F7" s="35" t="s">
         <v>115</v>
       </c>
-      <c r="G7" s="36" t="s">
+      <c r="G7" s="35" t="s">
         <v>115</v>
       </c>
       <c r="H7" s="14" t="s">

</xml_diff>